<commit_message>
Se actualiza documento de riesgos.
</commit_message>
<xml_diff>
--- a/1 - Planeacion/2 - Estrategia/Plan de riesgos.xlsx
+++ b/1 - Planeacion/2 - Estrategia/Plan de riesgos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>La ausencia de uno de los integrantes por fuerza mayor.</t>
   </si>
@@ -115,13 +115,22 @@
   </si>
   <si>
     <t>Retroalimentacion y apoyo mutuo de integrantes con desarrollos que afecten en su caso de uso.</t>
+  </si>
+  <si>
+    <t>La no aseptacion de la propuesta de aceptacion de elaboracion del producto por parte  de cliente.</t>
+  </si>
+  <si>
+    <t>Replanteamiento de la propuesta según criticas del usuario.</t>
+  </si>
+  <si>
+    <t>Observacion de cada uno de los puntos dados por el usuario y generalizacion entre el equipo de los requerimientos del cliente.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +144,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -152,33 +169,271 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -189,7 +444,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E11" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E11" totalsRowShown="0" headerRowDxfId="0" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:E11"/>
   <tableColumns count="5">
     <tableColumn id="1" name="DESCRIPCION" dataDxfId="5"/>
@@ -490,170 +745,180 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="A2:E11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="183.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="58.85546875" customWidth="1"/>
     <col min="5" max="5" width="87.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32.25" customHeight="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="23.25" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="23.25" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="24.75" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="22.5" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="24" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="25.5" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>